<commit_message>
v15.0.0 DataSet.AddBehavior DataSet.QueryNTATS输出格式优化 DataSet.QueryNTS DataSet.TableQuery输出格式优化 BatchOirRegisterTiff文档更新 HeatmapSort LanearHeatmap LinearPca 更新输入接口GroupNtats VectorCosine
</commit_message>
<xml_diff>
--- a/+UniExp/查询表.xlsx
+++ b/+UniExp/查询表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhtmf\Documents\MATLAB\统一实验分析作图\+UniExp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79062C45-F5B0-4457-880C-7F992912A75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E928B9FB-6F13-410F-B1AF-2F33E76828A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
   <si>
     <t>Design</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,10 +43,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GroupIndex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Mouse</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -95,7 +91,31 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1:10,12:20</t>
+    <t>GroupName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1:10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light_water_navie</t>
+  </si>
+  <si>
+    <t>Light_water_navie</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light_water_learned</t>
+  </si>
+  <si>
+    <t>Audio_water_transfer</t>
+  </si>
+  <si>
+    <t>Audio_water_final</t>
+  </si>
+  <si>
+    <t>First_10_trials</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -430,14 +450,15 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="10.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.625" style="1" customWidth="1"/>
     <col min="6" max="6" width="50.625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -452,18 +473,18 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -471,17 +492,17 @@
       <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -489,53 +510,53 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1">
-        <v>2</v>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="E5" s="1">
-        <v>4</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="1">
         <v>2</v>
@@ -543,53 +564,53 @@
       <c r="D6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1">
-        <v>2</v>
+      <c r="E6" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1">
         <v>1</v>
@@ -597,17 +618,17 @@
       <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="1">
-        <v>1</v>
+      <c r="E9" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
@@ -615,47 +636,47 @@
       <c r="D10" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="1">
-        <v>2</v>
+      <c r="E10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" s="1"/>
     </row>
@@ -666,8 +687,8 @@
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="1">
-        <v>5</v>
+      <c r="E13" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
更新数据格式：QueryNTATS ColorfulMarkerPlot HeatmapSort LanearHeatmap LinearPca
</commit_message>
<xml_diff>
--- a/+UniExp/查询表.xlsx
+++ b/+UniExp/查询表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhtmf\Documents\MATLAB\统一实验分析作图\+UniExp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Data-Server-1\个人数据\张天夫\202305\处理分析\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E928B9FB-6F13-410F-B1AF-2F33E76828A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE198AA-C5BA-40B3-B1BF-16F66F709FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
   <si>
     <t>Design</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -47,6 +47,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ZLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>LLw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -71,23 +75,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lhs1010,vtf0045,yqn0051</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LAuWLw</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>yqn2005,yqn3000,yqn3001,yqn3002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>vtf0030,yqn0022,lhs1010,vtf0045,yqn0051</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TrialIndex</t>
+    <t>WaterOnly</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LAuW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yqn2005,yqn3000,yqn3001,yqn3002,yqn2003,yqn1002,yqn1001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lhs1010,vtf0045,yqn0051,yqn0052</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>vtf0030,yqn0022,lhs1010,vtf0045,yqn0051,yqn0052</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -95,27 +103,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1:10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Light_water_navie</t>
-  </si>
-  <si>
-    <t>Light_water_navie</t>
+    <t>Water_only_naive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Light_water_naive</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Light_water_learned</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Audio_water_transfer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Audio_water_final</t>
-  </si>
-  <si>
-    <t>First_10_trials</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -159,12 +163,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -447,255 +448,279 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="50.625" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="4" width="10.625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="100.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>2</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1">
-        <v>2</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="1">
+      <c r="B9" s="1">
+        <v>2</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1">
+      <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F14" s="2"/>
+      <c r="E15" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
20240703 DataSet.AddBehavior：HitMiss支持表格输入 ReadQueryTable：支持合并单元格 TrialwiseEventPlot：ExcludedEvents改为名称值参数，额外支持指定ExcludedTrials
</commit_message>
<xml_diff>
--- a/+UniExp/查询表.xlsx
+++ b/+UniExp/查询表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Data-Server-1\个人数据\张天夫\202305\处理分析\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vhtmf\Documents\MATLAB\统一实验分析作图\+UniExp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE198AA-C5BA-40B3-B1BF-16F66F709FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9C872BA-94B7-4B95-8A9A-7BA77DA28073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Design</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -163,10 +163,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,7 +454,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -488,13 +491,13 @@
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -505,15 +508,9 @@
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="1">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
@@ -522,10 +519,8 @@
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -542,106 +537,82 @@
       <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C5" s="2"/>
       <c r="D5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="C7" s="2"/>
       <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1">
-        <v>2</v>
-      </c>
+      <c r="B8" s="2"/>
       <c r="C8" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="1">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="C10" s="2"/>
       <c r="D10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -650,79 +621,74 @@
       <c r="D11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
       <c r="D13" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="1">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="1">
         <v>2</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="C15" s="2"/>
       <c r="D15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="E15" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="E11:E15"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="B7:B9"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>